<commit_message>
add events to the import script
</commit_message>
<xml_diff>
--- a/scripts/Import Data.xlsx
+++ b/scripts/Import Data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="570" windowWidth="17895" windowHeight="9150" activeTab="1"/>
+    <workbookView xWindow="510" yWindow="570" windowWidth="17895" windowHeight="9150" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="1" r:id="rId1"/>
-    <sheet name="IMPORT SHEET" sheetId="2" r:id="rId2"/>
+    <sheet name="Users Import Queries" sheetId="2" r:id="rId2"/>
+    <sheet name="Events Import Queries" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
   <si>
     <t>This spreadsheet is an example of an easy, non-programmatic way to load data into Neo4j. Please copy, enhance and redistribute as much as you can.</t>
   </si>
@@ -141,71 +142,89 @@
     <t>Jarvis Noland</t>
   </si>
   <si>
-    <t>create n={id:'1', name:'Amada Emory'};</t>
-  </si>
-  <si>
-    <t>create n={id:'2', name:'Rana Seely'};</t>
-  </si>
-  <si>
-    <t>create n={id:'3', name:'Detra Thatcher'};</t>
-  </si>
-  <si>
-    <t>create n={id:'4', name:'Melda Reza'};</t>
-  </si>
-  <si>
-    <t>create n={id:'5', name:'Shana Willems'};</t>
-  </si>
-  <si>
-    <t>create n={id:'6', name:'Sharonda Peele'};</t>
-  </si>
-  <si>
-    <t>create n={id:'7', name:'Dagny Agee'};</t>
-  </si>
-  <si>
-    <t>create n={id:'8', name:'Tisa Woodman'};</t>
-  </si>
-  <si>
-    <t>create n={id:'9', name:'Shelba Mutchler'};</t>
-  </si>
-  <si>
-    <t>create n={id:'10', name:'Anderson Spagnola'};</t>
-  </si>
-  <si>
-    <t>create n={id:'11', name:'Pamala Forward'};</t>
-  </si>
-  <si>
-    <t>create n={id:'12', name:'Melva Fairchild'};</t>
-  </si>
-  <si>
-    <t>create n={id:'13', name:'Antione Selman'};</t>
-  </si>
-  <si>
-    <t>create n={id:'14', name:'Carmelia Cali'};</t>
-  </si>
-  <si>
-    <t>create n={id:'15', name:'Fairy Daughtery'};</t>
-  </si>
-  <si>
-    <t>create n={id:'16', name:'Stefany Mcamis'};</t>
-  </si>
-  <si>
-    <t>create n={id:'17', name:'Kermit Meaney'};</t>
-  </si>
-  <si>
-    <t>create n={id:'18', name:'Williemae Dossantos'};</t>
-  </si>
-  <si>
-    <t>create n={id:'19', name:'Marth Sparling'};</t>
-  </si>
-  <si>
-    <t>create n={id:'20', name:'Jarvis Noland'};</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>Bumble Bee Foods 5K</t>
+  </si>
+  <si>
+    <t>5K Zombie Run</t>
+  </si>
+  <si>
+    <t>Shelter Island 5K Run</t>
+  </si>
+  <si>
+    <t>New Me 5K &amp; 1Mile Kids Run</t>
+  </si>
+  <si>
+    <t>Finish Chelsea's Run 5K Run &amp; Walk</t>
+  </si>
+  <si>
+    <t>Cycling</t>
+  </si>
+  <si>
+    <t>PLRC Jim Krause Memorial Bicycle Ride</t>
+  </si>
+  <si>
+    <t>Templeton Wine &amp; Roses Bike Ride</t>
+  </si>
+  <si>
+    <t>Unddfeated EOD Bike Ride (Worldwide)</t>
+  </si>
+  <si>
+    <t>Campagnoio GranFondo San Diego 2014</t>
+  </si>
+  <si>
+    <t>Senorita Century - San Diego, Women's Bike Ride 2014</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>La Jolla 10 Mile Relay</t>
+  </si>
+  <si>
+    <t>Del Mar Relay Team Swim Meet</t>
+  </si>
+  <si>
+    <t>San Diego Swim Meetup</t>
+  </si>
+  <si>
+    <t>Coronado Freestyle Competition</t>
+  </si>
+  <si>
+    <t>San Diego Backstroke Meetup</t>
+  </si>
+  <si>
+    <t>San Diego Javascript Meetup</t>
+  </si>
+  <si>
+    <t>San Diego Ruby Meetup Night</t>
+  </si>
+  <si>
+    <t>Mac World 2014</t>
+  </si>
+  <si>
+    <t>Meetup</t>
+  </si>
+  <si>
+    <t>San Diego Startup Weekend 2014</t>
+  </si>
+  <si>
+    <t>San Diego RefreshSD</t>
+  </si>
+  <si>
+    <t>REGISTERED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -214,6 +233,12 @@
     <font>
       <b/>
       <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -703,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -719,10 +744,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -734,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -743,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -752,16 +777,16 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -782,19 +807,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -809,10 +834,19 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1294,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1340,8 +1374,9 @@
       <c r="B2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>41</v>
+      <c r="C2" s="17" t="str">
+        <f>"create n={id:'"&amp;A2&amp;"', name:'"&amp;B2&amp;"'};"</f>
+        <v>create n={id:'1', name:'Amada Emory'};</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1364,8 +1399,9 @@
       <c r="B3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>42</v>
+      <c r="C3" s="17" t="str">
+        <f>"create n={id:'"&amp;A3&amp;"', name:'"&amp;B3&amp;"'};"</f>
+        <v>create n={id:'2', name:'Rana Seely'};</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1388,8 +1424,9 @@
       <c r="B4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>43</v>
+      <c r="C4" s="17" t="str">
+        <f t="shared" ref="C3:C21" si="1">"create n={id:'"&amp;A4&amp;"', name:'"&amp;B4&amp;"'};"</f>
+        <v>create n={id:'3', name:'Detra Thatcher'};</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1412,8 +1449,9 @@
       <c r="B5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>44</v>
+      <c r="C5" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'4', name:'Melda Reza'};</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1436,8 +1474,9 @@
       <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>45</v>
+      <c r="C6" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'5', name:'Shana Willems'};</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1460,8 +1499,9 @@
       <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>46</v>
+      <c r="C7" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'6', name:'Sharonda Peele'};</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1484,8 +1524,9 @@
       <c r="B8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>47</v>
+      <c r="C8" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'7', name:'Dagny Agee'};</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -1508,8 +1549,9 @@
       <c r="B9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>48</v>
+      <c r="C9" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'8', name:'Tisa Woodman'};</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1532,8 +1574,9 @@
       <c r="B10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>49</v>
+      <c r="C10" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'9', name:'Shelba Mutchler'};</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1556,8 +1599,9 @@
       <c r="B11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>50</v>
+      <c r="C11" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'10', name:'Anderson Spagnola'};</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1580,8 +1624,9 @@
       <c r="B12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>51</v>
+      <c r="C12" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'11', name:'Pamala Forward'};</v>
       </c>
       <c r="E12">
         <v>14</v>
@@ -1604,8 +1649,9 @@
       <c r="B13" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>52</v>
+      <c r="C13" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'12', name:'Melva Fairchild'};</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -1628,8 +1674,9 @@
       <c r="B14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>53</v>
+      <c r="C14" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'13', name:'Antione Selman'};</v>
       </c>
       <c r="E14">
         <v>11</v>
@@ -1652,8 +1699,9 @@
       <c r="B15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>54</v>
+      <c r="C15" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'14', name:'Carmelia Cali'};</v>
       </c>
       <c r="E15">
         <v>12</v>
@@ -1676,8 +1724,9 @@
       <c r="B16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>55</v>
+      <c r="C16" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'15', name:'Fairy Daughtery'};</v>
       </c>
       <c r="E16">
         <v>12</v>
@@ -1700,8 +1749,9 @@
       <c r="B17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>56</v>
+      <c r="C17" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'16', name:'Stefany Mcamis'};</v>
       </c>
       <c r="E17">
         <v>12</v>
@@ -1724,8 +1774,9 @@
       <c r="B18" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>57</v>
+      <c r="C18" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'17', name:'Kermit Meaney'};</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1748,8 +1799,9 @@
       <c r="B19" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>58</v>
+      <c r="C19" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'18', name:'Williemae Dossantos'};</v>
       </c>
       <c r="E19">
         <v>13</v>
@@ -1772,8 +1824,9 @@
       <c r="B20" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>59</v>
+      <c r="C20" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'19', name:'Marth Sparling'};</v>
       </c>
       <c r="E20">
         <v>13</v>
@@ -1796,8 +1849,9 @@
       <c r="B21" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>60</v>
+      <c r="C21" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'20', name:'Jarvis Noland'};</v>
       </c>
       <c r="E21">
         <v>20</v>
@@ -1824,4 +1878,625 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="4" max="4" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="154.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="17" t="str">
+        <f>"create n={id:'"&amp;A2&amp;"', name:'"&amp;C2&amp;"', category:'"&amp;B2&amp;"'};"</f>
+        <v>create n={id:'1000', name:'Bumble Bee Foods 5K', category:'5K'};</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="9" t="str">
+        <f t="shared" ref="I2:I21" si="0">((((("start n1=node("&amp;F2)&amp;"),n2=node(")&amp;G2)&amp;") create n1-[:")&amp;H2)&amp;"]-&gt;n2;"</f>
+        <v>start n1=node(1),n2=node(1000) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>1001</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="17" t="str">
+        <f t="shared" ref="D3:D21" si="1">"create n={id:'"&amp;A3&amp;"', name:'"&amp;C3&amp;"', category:'"&amp;B3&amp;"'};"</f>
+        <v>create n={id:'1001', name:'5K Zombie Run', category:'5K'};</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(1),n2=node(1001) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>1002</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1002', name:'Shelter Island 5K Run', category:'5K'};</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1005</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(1),n2=node(1005) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>1003</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1003', name:'New Me 5K &amp; 1Mile Kids Run', category:'5K'};</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(2),n2=node(1000) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>1004</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1004', name:'Finish Chelsea's Run 5K Run &amp; Walk', category:'5K'};</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1010</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(2),n2=node(1010) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
+        <v>1005</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1005', name:'PLRC Jim Krause Memorial Bicycle Ride', category:'Cycling'};</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1009</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(2),n2=node(1009) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>1006</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1006', name:'Templeton Wine &amp; Roses Bike Ride', category:'Cycling'};</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>1019</v>
+      </c>
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(3),n2=node(1019) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
+        <v>1007</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1007', name:'Unddfeated EOD Bike Ride (Worldwide)', category:'Cycling'};</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>1017</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(3),n2=node(1017) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>1008</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1008', name:'Campagnoio GranFondo San Diego 2014', category:'Cycling'};</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>1003</v>
+      </c>
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(3),n2=node(1003) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="25">
+        <v>1009</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1009', name:'Senorita Century - San Diego, Women's Bike Ride 2014', category:'Cycling'};</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>1008</v>
+      </c>
+      <c r="H11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(10),n2=node(1008) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="25">
+        <v>1010</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1010', name:'La Jolla 10 Mile Relay', category:'Swimming'};</v>
+      </c>
+      <c r="F12">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>1004</v>
+      </c>
+      <c r="H12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(14),n2=node(1004) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="25">
+        <v>1011</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1011', name:'Del Mar Relay Team Swim Meet', category:'Swimming'};</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="H13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(11),n2=node(1000) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="25">
+        <v>1012</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1012', name:'San Diego Swim Meetup', category:'Swimming'};</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>1015</v>
+      </c>
+      <c r="H14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(11),n2=node(1015) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="25">
+        <v>1013</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1013', name:'Coronado Freestyle Competition', category:'Swimming'};</v>
+      </c>
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>1001</v>
+      </c>
+      <c r="H15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(12),n2=node(1001) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="25">
+        <v>1014</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1014', name:'San Diego Backstroke Meetup', category:'Swimming'};</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>1004</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(12),n2=node(1004) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="25">
+        <v>1015</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1015', name:'San Diego Javascript Meetup', category:'Meetup'};</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>1016</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(12),n2=node(1016) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="25">
+        <v>1016</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1016', name:'San Diego Ruby Meetup Night', category:'Meetup'};</v>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>1003</v>
+      </c>
+      <c r="H18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(17),n2=node(1003) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="25">
+        <v>1017</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1017', name:'Mac World 2014', category:'Meetup'};</v>
+      </c>
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>1003</v>
+      </c>
+      <c r="H19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(13),n2=node(1003) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="25">
+        <v>1018</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1018', name:'San Diego Startup Weekend 2014', category:'Meetup'};</v>
+      </c>
+      <c r="F20">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>1004</v>
+      </c>
+      <c r="H20" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(13),n2=node(1004) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="25">
+        <v>1019</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'1019', name:'San Diego RefreshSD', category:'Meetup'};</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>1011</v>
+      </c>
+      <c r="H21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(20),n2=node(1011) create n1-[:REGISTERED]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="25"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
making it rain registrations!
</commit_message>
<xml_diff>
--- a/scripts/Import Data.xlsx
+++ b/scripts/Import Data.xlsx
@@ -160,9 +160,6 @@
     <t>New Me 5K &amp; 1Mile Kids Run</t>
   </si>
   <si>
-    <t>Finish Chelsea's Run 5K Run &amp; Walk</t>
-  </si>
-  <si>
     <t>Cycling</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>Campagnoio GranFondo San Diego 2014</t>
   </si>
   <si>
-    <t>Senorita Century - San Diego, Women's Bike Ride 2014</t>
-  </si>
-  <si>
     <t>Swimming</t>
   </si>
   <si>
@@ -218,6 +212,12 @@
   </si>
   <si>
     <t>REGISTERED</t>
+  </si>
+  <si>
+    <t>Finish Chelseas Run 5K Run &amp; Walk</t>
+  </si>
+  <si>
+    <t>Senorita Century - San Diego, Womens Bike Ride 2014</t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1948,7 +1948,7 @@
         <v>1000</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I2" s="9" t="str">
         <f t="shared" ref="I2:I21" si="0">((((("start n1=node("&amp;F2)&amp;"),n2=node(")&amp;G2)&amp;") create n1-[:")&amp;H2)&amp;"]-&gt;n2;"</f>
@@ -1976,7 +1976,7 @@
         <v>1001</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2004,7 +2004,7 @@
         <v>1005</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I4" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2032,7 +2032,7 @@
         <v>1000</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I5" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2047,11 +2047,11 @@
         <v>42</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="D6" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1004', name:'Finish Chelsea's Run 5K Run &amp; Walk', category:'5K'};</v>
+        <v>create n={id:'1004', name:'Finish Chelseas Run 5K Run &amp; Walk', category:'5K'};</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -2060,7 +2060,7 @@
         <v>1010</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I6" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2072,10 +2072,10 @@
         <v>1005</v>
       </c>
       <c r="B7" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>49</v>
       </c>
       <c r="D7" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2088,7 +2088,7 @@
         <v>1009</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I7" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2100,10 +2100,10 @@
         <v>1006</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2116,7 +2116,7 @@
         <v>1019</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I8" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2128,10 +2128,10 @@
         <v>1007</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2144,7 +2144,7 @@
         <v>1017</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I9" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2156,10 +2156,10 @@
         <v>1008</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2172,7 +2172,7 @@
         <v>1003</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I10" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2184,14 +2184,14 @@
         <v>1009</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D11" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1009', name:'Senorita Century - San Diego, Women's Bike Ride 2014', category:'Cycling'};</v>
+        <v>create n={id:'1009', name:'Senorita Century - San Diego, Womens Bike Ride 2014', category:'Cycling'};</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -2200,7 +2200,7 @@
         <v>1008</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I11" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2212,10 +2212,10 @@
         <v>1010</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2228,7 +2228,7 @@
         <v>1004</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I12" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2240,10 +2240,10 @@
         <v>1011</v>
       </c>
       <c r="B13" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="39" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>56</v>
       </c>
       <c r="D13" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2256,7 +2256,7 @@
         <v>1000</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I13" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2268,10 +2268,10 @@
         <v>1012</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2284,7 +2284,7 @@
         <v>1015</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I14" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2296,10 +2296,10 @@
         <v>1013</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2312,7 +2312,7 @@
         <v>1001</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I15" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2324,10 +2324,10 @@
         <v>1014</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2340,7 +2340,7 @@
         <v>1004</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I16" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2352,10 +2352,10 @@
         <v>1015</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2368,7 +2368,7 @@
         <v>1016</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I17" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2380,10 +2380,10 @@
         <v>1016</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2396,7 +2396,7 @@
         <v>1003</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I18" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2408,10 +2408,10 @@
         <v>1017</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2424,7 +2424,7 @@
         <v>1003</v>
       </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I19" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2436,10 +2436,10 @@
         <v>1018</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2452,7 +2452,7 @@
         <v>1004</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I20" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2464,10 +2464,10 @@
         <v>1019</v>
       </c>
       <c r="B21" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="39" t="s">
         <v>63</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>65</v>
       </c>
       <c r="D21" s="17" t="str">
         <f t="shared" si="1"/>
@@ -2480,7 +2480,7 @@
         <v>1011</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" s="9" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Add interests sucka's! Woot!
</commit_message>
<xml_diff>
--- a/scripts/Import Data.xlsx
+++ b/scripts/Import Data.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="570" windowWidth="17895" windowHeight="9150" activeTab="2"/>
+    <workbookView xWindow="510" yWindow="570" windowWidth="17895" windowHeight="9150" tabRatio="607" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9555" windowHeight="7740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="1" r:id="rId1"/>
     <sheet name="Users Import Queries" sheetId="2" r:id="rId2"/>
     <sheet name="Events Import Queries" sheetId="3" r:id="rId3"/>
+    <sheet name="Interests Import Queries" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="78">
   <si>
     <t>This spreadsheet is an example of an easy, non-programmatic way to load data into Neo4j. Please copy, enhance and redistribute as much as you can.</t>
   </si>
@@ -163,9 +164,6 @@
     <t>Cycling</t>
   </si>
   <si>
-    <t>PLRC Jim Krause Memorial Bicycle Ride</t>
-  </si>
-  <si>
     <t>Templeton Wine &amp; Roses Bike Ride</t>
   </si>
   <si>
@@ -208,9 +206,6 @@
     <t>San Diego Startup Weekend 2014</t>
   </si>
   <si>
-    <t>San Diego RefreshSD</t>
-  </si>
-  <si>
     <t>REGISTERED</t>
   </si>
   <si>
@@ -218,6 +213,45 @@
   </si>
   <si>
     <t>Senorita Century - San Diego, Womens Bike Ride 2014</t>
+  </si>
+  <si>
+    <t>Running a 5K</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Apple Products</t>
+  </si>
+  <si>
+    <t>Wine</t>
+  </si>
+  <si>
+    <t>Riding a road bike</t>
+  </si>
+  <si>
+    <t>Zombies</t>
+  </si>
+  <si>
+    <t>Womens Groups</t>
+  </si>
+  <si>
+    <t>Start  Ups</t>
+  </si>
+  <si>
+    <t>Jim Krause Memorial Bicycle Ride</t>
+  </si>
+  <si>
+    <t>San Diego ComicCon 2014</t>
+  </si>
+  <si>
+    <t>Comics</t>
+  </si>
+  <si>
+    <t>Playing the Drums</t>
+  </si>
+  <si>
+    <t>RELATED_TO</t>
   </si>
 </sst>
 </file>
@@ -834,19 +868,19 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1190,6 +1224,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1198,7 +1233,7 @@
     <col min="3" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1252,11 +1287,11 @@
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1310,7 +1345,7 @@
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>13</v>
       </c>
@@ -1329,8 +1364,9 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1425,7 +1461,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="17" t="str">
-        <f t="shared" ref="C3:C21" si="1">"create n={id:'"&amp;A4&amp;"', name:'"&amp;B4&amp;"'};"</f>
+        <f t="shared" ref="C4:C21" si="1">"create n={id:'"&amp;A4&amp;"', name:'"&amp;B4&amp;"'};"</f>
         <v>create n={id:'3', name:'Detra Thatcher'};</v>
       </c>
       <c r="E4">
@@ -1884,9 +1920,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1904,7 +1941,7 @@
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>41</v>
       </c>
       <c r="C1" s="34" t="s">
@@ -1929,567 +1966,567 @@
     </row>
     <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25">
-        <v>1000</v>
-      </c>
-      <c r="B2" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="17" t="str">
         <f>"create n={id:'"&amp;A2&amp;"', name:'"&amp;C2&amp;"', category:'"&amp;B2&amp;"'};"</f>
-        <v>create n={id:'1000', name:'Bumble Bee Foods 5K', category:'5K'};</v>
+        <v>create n={id:'21', name:'Bumble Bee Foods 5K', category:'5K'};</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1000</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I2" s="9" t="str">
         <f t="shared" ref="I2:I21" si="0">((((("start n1=node("&amp;F2)&amp;"),n2=node(")&amp;G2)&amp;") create n1-[:")&amp;H2)&amp;"]-&gt;n2;"</f>
-        <v>start n1=node(1),n2=node(1000) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(1),n2=node(21) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25">
-        <v>1001</v>
-      </c>
-      <c r="B3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="37" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="17" t="str">
         <f t="shared" ref="D3:D21" si="1">"create n={id:'"&amp;A3&amp;"', name:'"&amp;C3&amp;"', category:'"&amp;B3&amp;"'};"</f>
-        <v>create n={id:'1001', name:'5K Zombie Run', category:'5K'};</v>
+        <v>create n={id:'22', name:'5K Zombie Run', category:'5K'};</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1001</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I3" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(1),n2=node(1001) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(1),n2=node(22) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
-        <v>1002</v>
-      </c>
-      <c r="B4" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="37" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1002', name:'Shelter Island 5K Run', category:'5K'};</v>
+        <v>create n={id:'23', name:'Shelter Island 5K Run', category:'5K'};</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1005</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I4" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(1),n2=node(1005) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(1),n2=node(25) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25">
-        <v>1003</v>
-      </c>
-      <c r="B5" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="37" t="s">
         <v>46</v>
       </c>
       <c r="D5" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1003', name:'New Me 5K &amp; 1Mile Kids Run', category:'5K'};</v>
+        <v>create n={id:'24', name:'New Me 5K &amp; 1Mile Kids Run', category:'5K'};</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5">
-        <v>1000</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I5" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(2),n2=node(1000) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(2),n2=node(21) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
-        <v>1004</v>
-      </c>
-      <c r="B6" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>65</v>
+      <c r="C6" s="37" t="s">
+        <v>63</v>
       </c>
       <c r="D6" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1004', name:'Finish Chelseas Run 5K Run &amp; Walk', category:'5K'};</v>
+        <v>create n={id:'25', name:'Finish Chelseas Run 5K Run &amp; Walk', category:'5K'};</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <v>1010</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I6" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(2),n2=node(1010) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(2),n2=node(30) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25">
-        <v>1005</v>
-      </c>
-      <c r="B7" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>48</v>
+      <c r="C7" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="D7" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1005', name:'PLRC Jim Krause Memorial Bicycle Ride', category:'Cycling'};</v>
+        <v>create n={id:'26', name:'Jim Krause Memorial Bicycle Ride', category:'Cycling'};</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>1009</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(2),n2=node(1009) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(2),n2=node(29) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25">
-        <v>1006</v>
-      </c>
-      <c r="B8" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="39" t="s">
-        <v>49</v>
+      <c r="C8" s="37" t="s">
+        <v>48</v>
       </c>
       <c r="D8" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1006', name:'Templeton Wine &amp; Roses Bike Ride', category:'Cycling'};</v>
+        <v>create n={id:'27', name:'Templeton Wine &amp; Roses Bike Ride', category:'Cycling'};</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8">
-        <v>1019</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(3),n2=node(1019) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(3),n2=node(39) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25">
-        <v>1007</v>
-      </c>
-      <c r="B9" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>50</v>
+      <c r="C9" s="37" t="s">
+        <v>49</v>
       </c>
       <c r="D9" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1007', name:'Unddfeated EOD Bike Ride (Worldwide)', category:'Cycling'};</v>
+        <v>create n={id:'28', name:'Unddfeated EOD Bike Ride (Worldwide)', category:'Cycling'};</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9">
-        <v>1017</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(3),n2=node(1017) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(3),n2=node(37) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
-        <v>1008</v>
-      </c>
-      <c r="B10" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>51</v>
+      <c r="C10" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="D10" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1008', name:'Campagnoio GranFondo San Diego 2014', category:'Cycling'};</v>
+        <v>create n={id:'29', name:'Campagnoio GranFondo San Diego 2014', category:'Cycling'};</v>
       </c>
       <c r="F10">
         <v>3</v>
       </c>
       <c r="G10">
-        <v>1003</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(3),n2=node(1003) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(3),n2=node(34) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="25">
-        <v>1009</v>
-      </c>
-      <c r="B11" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>66</v>
+      <c r="C11" s="37" t="s">
+        <v>64</v>
       </c>
       <c r="D11" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1009', name:'Senorita Century - San Diego, Womens Bike Ride 2014', category:'Cycling'};</v>
+        <v>create n={id:'30', name:'Senorita Century - San Diego, Womens Bike Ride 2014', category:'Cycling'};</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11">
-        <v>1008</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I11" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(10),n2=node(1008) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(10),n2=node(29) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="25">
-        <v>1010</v>
-      </c>
-      <c r="B12" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="39" t="s">
-        <v>53</v>
-      </c>
       <c r="D12" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1010', name:'La Jolla 10 Mile Relay', category:'Swimming'};</v>
+        <v>create n={id:'31', name:'La Jolla 10 Mile Relay', category:'Swimming'};</v>
       </c>
       <c r="F12">
         <v>14</v>
       </c>
       <c r="G12">
-        <v>1004</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I12" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(14),n2=node(1004) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(14),n2=node(25) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="25">
-        <v>1011</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>54</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>53</v>
       </c>
       <c r="D13" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1011', name:'Del Mar Relay Team Swim Meet', category:'Swimming'};</v>
+        <v>create n={id:'32', name:'Del Mar Relay Team Swim Meet', category:'Swimming'};</v>
       </c>
       <c r="F13">
         <v>11</v>
       </c>
       <c r="G13">
-        <v>1000</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I13" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(11),n2=node(1000) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(11),n2=node(21) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="25">
-        <v>1012</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>54</v>
       </c>
       <c r="D14" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1012', name:'San Diego Swim Meetup', category:'Swimming'};</v>
+        <v>create n={id:'33', name:'San Diego Swim Meetup', category:'Swimming'};</v>
       </c>
       <c r="F14">
         <v>11</v>
       </c>
       <c r="G14">
-        <v>1015</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I14" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(11),n2=node(1015) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(11),n2=node(36) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="25">
-        <v>1013</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>56</v>
+        <v>34</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>55</v>
       </c>
       <c r="D15" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1013', name:'Coronado Freestyle Competition', category:'Swimming'};</v>
+        <v>create n={id:'34', name:'Coronado Freestyle Competition', category:'Swimming'};</v>
       </c>
       <c r="F15">
         <v>12</v>
       </c>
       <c r="G15">
-        <v>1001</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I15" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(12),n2=node(1001) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(12),n2=node(22) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="25">
-        <v>1014</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>56</v>
       </c>
       <c r="D16" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1014', name:'San Diego Backstroke Meetup', category:'Swimming'};</v>
+        <v>create n={id:'35', name:'San Diego Backstroke Meetup', category:'Swimming'};</v>
       </c>
       <c r="F16">
         <v>12</v>
       </c>
       <c r="G16">
-        <v>1004</v>
+        <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I16" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(12),n2=node(1004) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(12),n2=node(25) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="25">
-        <v>1015</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>58</v>
+        <v>36</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>57</v>
       </c>
       <c r="D17" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1015', name:'San Diego Javascript Meetup', category:'Meetup'};</v>
+        <v>create n={id:'36', name:'San Diego Javascript Meetup', category:'Meetup'};</v>
       </c>
       <c r="F17">
         <v>12</v>
       </c>
       <c r="G17">
-        <v>1016</v>
+        <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I17" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(12),n2=node(1016) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(12),n2=node(37) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
-        <v>1016</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>59</v>
+        <v>37</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>58</v>
       </c>
       <c r="D18" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1016', name:'San Diego Ruby Meetup Night', category:'Meetup'};</v>
+        <v>create n={id:'37', name:'San Diego Ruby Meetup Night', category:'Meetup'};</v>
       </c>
       <c r="F18">
         <v>17</v>
       </c>
       <c r="G18">
-        <v>1003</v>
+        <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I18" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(17),n2=node(1003) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(17),n2=node(24) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="25">
-        <v>1017</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>60</v>
       </c>
+      <c r="C19" s="37" t="s">
+        <v>59</v>
+      </c>
       <c r="D19" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1017', name:'Mac World 2014', category:'Meetup'};</v>
+        <v>create n={id:'38', name:'Mac World 2014', category:'Meetup'};</v>
       </c>
       <c r="F19">
         <v>13</v>
       </c>
       <c r="G19">
-        <v>1003</v>
+        <v>24</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I19" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(13),n2=node(1003) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(13),n2=node(24) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="25">
-        <v>1018</v>
-      </c>
-      <c r="B20" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="39" t="s">
-        <v>62</v>
-      </c>
       <c r="D20" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1018', name:'San Diego Startup Weekend 2014', category:'Meetup'};</v>
+        <v>create n={id:'39', name:'San Diego Startup Weekend 2014', category:'Meetup'};</v>
       </c>
       <c r="F20">
         <v>13</v>
       </c>
       <c r="G20">
-        <v>1004</v>
+        <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I20" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(13),n2=node(1004) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(13),n2=node(25) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="25">
-        <v>1019</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>74</v>
       </c>
       <c r="D21" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>create n={id:'1019', name:'San Diego RefreshSD', category:'Meetup'};</v>
+        <v>create n={id:'40', name:'San Diego ComicCon 2014', category:'Meetup'};</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
       <c r="G21">
-        <v>1011</v>
+        <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>start n1=node(20),n2=node(1011) create n1-[:REGISTERED]-&gt;n2;</v>
+        <v>start n1=node(20),n2=node(32) create n1-[:REGISTERED]-&gt;n2;</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="25"/>
-      <c r="B22" s="38"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="24"/>
       <c r="D22" s="11"/>
       <c r="E22" s="32"/>
@@ -2499,4 +2536,455 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="1">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="154.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>41</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="17" t="str">
+        <f>"create n={id:'"&amp;A2&amp;"', name:'"&amp;B2&amp;"'};"</f>
+        <v>create n={id:'41', name:'Running a 5K'};</v>
+      </c>
+      <c r="E2">
+        <v>41</v>
+      </c>
+      <c r="F2">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="9" t="str">
+        <f t="shared" ref="H2:H11" si="0">((((("start n1=node("&amp;E2)&amp;"),n2=node(")&amp;F2)&amp;") create n1-[:")&amp;G2)&amp;"]-&gt;n2;"</f>
+        <v>start n1=node(41),n2=node(21) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>42</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="17" t="str">
+        <f t="shared" ref="C3:C11" si="1">"create n={id:'"&amp;A3&amp;"', name:'"&amp;B3&amp;"'};"</f>
+        <v>create n={id:'42', name:'Programming'};</v>
+      </c>
+      <c r="E3">
+        <v>41</v>
+      </c>
+      <c r="F3">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="9" t="str">
+        <f t="shared" ref="H3:H21" si="2">((((("start n1=node("&amp;E3)&amp;"),n2=node(")&amp;F3)&amp;") create n1-[:")&amp;G3)&amp;"]-&gt;n2;"</f>
+        <v>start n1=node(41),n2=node(22) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>43</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'43', name:'Apple Products'};</v>
+      </c>
+      <c r="E4">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(41),n2=node(23) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>44</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'44', name:'Wine'};</v>
+      </c>
+      <c r="E5">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(41),n2=node(24) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>45</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'45', name:'Riding a road bike'};</v>
+      </c>
+      <c r="E6">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(41),n2=node(25) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
+        <v>46</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'46', name:'Zombies'};</v>
+      </c>
+      <c r="E7">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(42),n2=node(36) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>47</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'47', name:'Womens Groups'};</v>
+      </c>
+      <c r="E8">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(42),n2=node(37) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
+        <v>48</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'48', name:'Start  Ups'};</v>
+      </c>
+      <c r="E9">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(42),n2=node(38) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>49</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'49', name:'Comics'};</v>
+      </c>
+      <c r="E10">
+        <v>42</v>
+      </c>
+      <c r="F10">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(42),n2=node(39) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="25">
+        <v>50</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'50', name:'Playing the Drums'};</v>
+      </c>
+      <c r="E11">
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(43),n2=node(38) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>44</v>
+      </c>
+      <c r="F12">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(44),n2=node(27) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(45),n2=node(26) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(45),n2=node(27) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(45),n2=node(28) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(45),n2=node(29) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(45),n2=node(30) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>46</v>
+      </c>
+      <c r="F18">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(46),n2=node(22) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>47</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(47),n2=node(30) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>48</v>
+      </c>
+      <c r="F20">
+        <v>39</v>
+      </c>
+      <c r="G20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(48),n2=node(39) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>49</v>
+      </c>
+      <c r="F21">
+        <v>40</v>
+      </c>
+      <c r="G21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(49),n2=node(40) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added relationships for users to interests
</commit_message>
<xml_diff>
--- a/scripts/Import Data.xlsx
+++ b/scripts/Import Data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="510" yWindow="570" windowWidth="17895" windowHeight="9150" tabRatio="607" firstSheet="2" activeTab="2"/>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9555" windowHeight="7740" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9555" windowHeight="7740" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="1" r:id="rId1"/>
     <sheet name="Users Import Queries" sheetId="2" r:id="rId2"/>
     <sheet name="Events Import Queries" sheetId="3" r:id="rId3"/>
-    <sheet name="Interests Import Queries" sheetId="4" r:id="rId4"/>
+    <sheet name="Interests-Events Import Queries" sheetId="4" r:id="rId4"/>
+    <sheet name="Interests-Users Import Queries" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="79">
   <si>
     <t>This spreadsheet is an example of an easy, non-programmatic way to load data into Neo4j. Please copy, enhance and redistribute as much as you can.</t>
   </si>
@@ -252,6 +253,9 @@
   </si>
   <si>
     <t>RELATED_TO</t>
+  </si>
+  <si>
+    <t>INTERESTED_IN</t>
   </si>
 </sst>
 </file>
@@ -1921,9 +1925,9 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2543,10 +2547,10 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="1">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="1">
+      <selection activeCell="C27" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2605,7 +2609,7 @@
         <v>77</v>
       </c>
       <c r="H2" s="9" t="str">
-        <f t="shared" ref="H2:H11" si="0">((((("start n1=node("&amp;E2)&amp;"),n2=node(")&amp;F2)&amp;") create n1-[:")&amp;G2)&amp;"]-&gt;n2;"</f>
+        <f t="shared" ref="H2" si="0">((((("start n1=node("&amp;E2)&amp;"),n2=node(")&amp;F2)&amp;") create n1-[:")&amp;G2)&amp;"]-&gt;n2;"</f>
         <v>start n1=node(41),n2=node(21) create n1-[:RELATED_TO]-&gt;n2;</v>
       </c>
     </row>
@@ -2982,6 +2986,533 @@
       <c r="H21" s="9" t="str">
         <f t="shared" si="2"/>
         <v>start n1=node(49),n2=node(40) create n1-[:RELATED_TO]-&gt;n2;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H26"/>
+    </sheetView>
+    <sheetView topLeftCell="A2" workbookViewId="1">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="154.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>41</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="17" t="str">
+        <f>"create n={id:'"&amp;A2&amp;"', name:'"&amp;B2&amp;"'};"</f>
+        <v>create n={id:'41', name:'Running a 5K'};</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="9" t="str">
+        <f t="shared" ref="H2:H21" si="0">((((("start n1=node("&amp;E2)&amp;"),n2=node(")&amp;F2)&amp;") create n1-[:")&amp;G2)&amp;"]-&gt;n2;"</f>
+        <v>start n1=node(1),n2=node(41) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>42</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="17" t="str">
+        <f t="shared" ref="C3:C11" si="1">"create n={id:'"&amp;A3&amp;"', name:'"&amp;B3&amp;"'};"</f>
+        <v>create n={id:'42', name:'Programming'};</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(1),n2=node(46) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>43</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'43', name:'Apple Products'};</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(2),n2=node(41) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>44</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'44', name:'Wine'};</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(2),n2=node(47) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>45</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'45', name:'Riding a road bike'};</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(2),n2=node(45) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
+        <v>46</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'46', name:'Zombies'};</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(3),n2=node(48) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>47</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'47', name:'Womens Groups'};</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(3),n2=node(42) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
+        <v>48</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'48', name:'Start  Ups'};</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(10),n2=node(45) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>49</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'49', name:'Comics'};</v>
+      </c>
+      <c r="E10">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(14),n2=node(41) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="25">
+        <v>50</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>create n={id:'50', name:'Playing the Drums'};</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(11),n2=node(41) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(11),n2=node(42) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(12),n2=node(41) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(12),n2=node(46) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(17),n2=node(41) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(13),n2=node(41) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(5),n2=node(42) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>49</v>
+      </c>
+      <c r="G18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(6),n2=node(49) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>49</v>
+      </c>
+      <c r="G19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(7),n2=node(49) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(8),n2=node(50) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>start n1=node(9),n2=node(50) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="9" t="str">
+        <f t="shared" ref="H22:H26" si="2">((((("start n1=node("&amp;E22)&amp;"),n2=node(")&amp;F22)&amp;") create n1-[:")&amp;G22)&amp;"]-&gt;n2;"</f>
+        <v>start n1=node(10),n2=node(50) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(11),n2=node(50) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(12),n2=node(50) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>13</v>
+      </c>
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(13),n2=node(50) create n1-[:INTERESTED_IN]-&gt;n2;</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>start n1=node(14),n2=node(50) create n1-[:INTERESTED_IN]-&gt;n2;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>